<commit_message>
OpenScenario okay for runnning experiments A and B
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/SSHConfig.xlsx
+++ b/AD-EYE/TA/SSHConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12B568F-98CB-4206-AA72-1E1113AB4FFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45AB5AD-891D-4AA6-94FD-37D93CDAD177}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>ipaddress</t>
   </si>
   <si>
-    <t>192.168.122.1</t>
-  </si>
-  <si>
     <t>user</t>
   </si>
   <si>
@@ -63,7 +60,10 @@
     <t>hostname</t>
   </si>
   <si>
-    <t>adeye06u</t>
+    <t>130.237.10.123</t>
+  </si>
+  <si>
+    <t>adeye03u</t>
   </si>
 </sst>
 </file>
@@ -418,13 +418,14 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -440,44 +441,44 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Saving files for ssh config (contact Maxime)
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/SSHConfig.xlsx
+++ b/AD-EYE/TA/SSHConfig.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45AB5AD-891D-4AA6-94FD-37D93CDAD177}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA245C0-AAC3-495D-BB28-067044F2D339}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,10 +60,10 @@
     <t>hostname</t>
   </si>
   <si>
-    <t>130.237.10.123</t>
-  </si>
-  <si>
-    <t>adeye03u</t>
+    <t>adeye06u</t>
+  </si>
+  <si>
+    <t>192.168.122.1</t>
   </si>
 </sst>
 </file>
@@ -418,7 +418,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +441,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -481,7 +481,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>